<commit_message>
random bug with googleMapsClient
</commit_message>
<xml_diff>
--- a/processed-excel_example.xlsx
+++ b/processed-excel_example.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -386,9 +386,6 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
-        <v>Address</v>
-      </c>
       <c r="B1" t="str">
         <v>Latitude</v>
       </c>
@@ -396,153 +393,10 @@
         <v>Longitude</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>1 Crossgates Mall Road</v>
-      </c>
-      <c r="B2" t="str">
-        <v>42.6893209</v>
-      </c>
-      <c r="C2" t="str">
-        <v>-73.8484059</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Duke Rd &amp; Walden Ave</v>
-      </c>
-      <c r="B3" t="str">
-        <v>42.9045546</v>
-      </c>
-      <c r="C3" t="str">
-        <v>-78.7575109</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>630 Old Country Rd.</v>
-      </c>
-      <c r="B4" t="str">
-        <v>40.7382095</v>
-      </c>
-      <c r="C4" t="str">
-        <v>-73.6143694</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>160 Walt Whitman Rd.</v>
-      </c>
-      <c r="B5" t="str">
-        <v>40.8229535</v>
-      </c>
-      <c r="C5" t="str">
-        <v>-73.4106588</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>1 Crossgates Mall Road</v>
-      </c>
-      <c r="B6" t="str">
-        <v>42.6893209</v>
-      </c>
-      <c r="C6" t="str">
-        <v>-73.8484059</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Duke Rd &amp; Walden Ave</v>
-      </c>
-      <c r="B7" t="str">
-        <v>42.9045546</v>
-      </c>
-      <c r="C7" t="str">
-        <v>-78.7575109</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>630 Old Country Rd.</v>
-      </c>
-      <c r="B8" t="str">
-        <v>40.7382095</v>
-      </c>
-      <c r="C8" t="str">
-        <v>-73.6143694</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>160 Walt Whitman Rd.</v>
-      </c>
-      <c r="B9" t="str">
-        <v>40.8229535</v>
-      </c>
-      <c r="C9" t="str">
-        <v>-73.4106588</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>1 Crossgates Mall Road</v>
-      </c>
-      <c r="B10" t="str">
-        <v>42.6893209</v>
-      </c>
-      <c r="C10" t="str">
-        <v>-73.8484059</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>Duke Rd &amp; Walden Ave</v>
-      </c>
-      <c r="B11" t="str">
-        <v>42.9045546</v>
-      </c>
-      <c r="C11" t="str">
-        <v>-78.7575109</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>630 Old Country Rd.</v>
-      </c>
-      <c r="B12" t="str">
-        <v>40.7382095</v>
-      </c>
-      <c r="C12" t="str">
-        <v>-73.6143694</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>160 Walt Whitman Rd.</v>
-      </c>
-      <c r="B13" t="str">
-        <v>40.8229535</v>
-      </c>
-      <c r="C13" t="str">
-        <v>-73.4106588</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>Matrix house Milton Keynes UK</v>
-      </c>
-      <c r="B14" t="str">
-        <v>52.0401578</v>
-      </c>
-      <c r="C14" t="str">
-        <v>-0.7697067999999999</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>